<commit_message>
feat(pdf): add template-based PDF generation with quarterly and yearly reports
- Add PDF template formatter for quarterly recap and statistics reports
- Implement new PDF generation methods using blade templates
- Add view location for PDF templates in AppServiceProvider
- Create blade templates for monthly, quarterly and yearly reports
- Update ExportService to use new template-based PDF generation
</commit_message>
<xml_diff>
--- a/resources/excel/puskesmas.xlsx
+++ b/resources/excel/puskesmas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Program\GitHub\akudihatinya\akudihatinya-backend\resources\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Program\GitHub\akudihatinya\akudihatinya-backend\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE89127A-56F2-4AC8-8AB5-E3158E20C6C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A654DA8-D6CF-4112-AB67-4C0D32C91016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{54DF6366-42DF-47E1-8A5D-3CF0032E5F84}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
   <si>
     <t>SASARAN</t>
   </si>
@@ -120,9 +120,6 @@
     <t>:</t>
   </si>
   <si>
-    <t>Pelayanan Kesehatan Pada Penderita Diabetes Melitus</t>
-  </si>
-  <si>
     <t>PUSKESMAS</t>
   </si>
   <si>
@@ -133,6 +130,15 @@
   </si>
   <si>
     <t>TOTAL CAPAIAN TAHUN &lt;tahun&gt;</t>
+  </si>
+  <si>
+    <t>Pelayanan Kesehatan Pada Penderita &lt;disease_type&gt;</t>
+  </si>
+  <si>
+    <t>&lt;mulai&gt;</t>
+  </si>
+  <si>
+    <t>&lt;rekap&gt;</t>
   </si>
 </sst>
 </file>
@@ -962,7 +968,7 @@
   <dimension ref="A1:BQ25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1050,7 +1056,7 @@
     </row>
     <row r="2" spans="1:69" s="1" customFormat="1" ht="21">
       <c r="A2" s="27" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B2" s="27"/>
       <c r="C2" s="27"/>
@@ -1200,7 +1206,7 @@
         <v>27</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -1214,13 +1220,13 @@
     </row>
     <row r="5" spans="1:69" s="1" customFormat="1" ht="21">
       <c r="A5" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>27</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
@@ -1248,7 +1254,7 @@
         <v>22</v>
       </c>
       <c r="H7" s="40" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I7" s="41"/>
       <c r="J7" s="41"/>
@@ -1290,7 +1296,9 @@
       <c r="A9" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="14"/>
+      <c r="B9" s="14" t="s">
+        <v>33</v>
+      </c>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
@@ -1317,7 +1325,9 @@
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
       <c r="F10" s="15"/>
-      <c r="H10" s="23"/>
+      <c r="H10" s="23" t="s">
+        <v>34</v>
+      </c>
       <c r="I10" s="23"/>
       <c r="J10" s="23"/>
       <c r="K10" s="23"/>

</xml_diff>

<commit_message>
refactor(export): consolidate puskesmas export functionality into statistics api
- Move puskesmas export routes and controller logic into statistics controller
- Update documentation to reflect consolidated endpoints
- Add puskesmas export support to existing statistics export endpoint
- Update test script for new endpoint structure
</commit_message>
<xml_diff>
--- a/resources/excel/puskesmas.xlsx
+++ b/resources/excel/puskesmas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Program\GitHub\akudihatinya\akudihatinya-backend\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A654DA8-D6CF-4112-AB67-4C0D32C91016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29025F66-9195-4BA9-8B25-4F765C15B9A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{54DF6366-42DF-47E1-8A5D-3CF0032E5F84}"/>
   </bookViews>
@@ -501,7 +501,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -607,6 +607,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="45">
     <cellStyle name="Comma [0] 2" xfId="1" xr:uid="{043EDEDA-AEEA-4E31-9086-8ABCA93B06A9}"/>
@@ -968,7 +969,7 @@
   <dimension ref="A1:BQ25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1205,10 +1206,10 @@
       <c r="B4" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="10"/>
+      <c r="D4" s="27"/>
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
@@ -1225,10 +1226,10 @@
       <c r="B5" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="10"/>
+      <c r="D5" s="43"/>
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
@@ -1570,7 +1571,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="A2:M2"/>
     <mergeCell ref="E7:E8"/>
@@ -1582,6 +1583,7 @@
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="H8:J8"/>
     <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C4:D4"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="256" scale="70" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>